<commit_message>
Type III reference submissions added.
</commit_message>
<xml_diff>
--- a/predictions/SAMPL6_user_map_pKa.xlsx
+++ b/predictions/SAMPL6_user_map_pKa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="25360" windowHeight="14200" tabRatio="500"/>
+    <workbookView xWindow="36640" yWindow="520" windowWidth="25360" windowHeight="14200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="284">
   <si>
     <t>firstname</t>
   </si>
@@ -817,16 +817,86 @@
   </si>
   <si>
     <t>y75vj-976-typeIII-NHLBI-5.csv</t>
+  </si>
+  <si>
+    <t>nb001</t>
+  </si>
+  <si>
+    <t>nb002</t>
+  </si>
+  <si>
+    <t>nb003</t>
+  </si>
+  <si>
+    <t>nb004</t>
+  </si>
+  <si>
+    <t>nb005</t>
+  </si>
+  <si>
+    <t>nb006</t>
+  </si>
+  <si>
+    <t>post-deadline</t>
+  </si>
+  <si>
+    <t>nb001-976-typeIII-ECRISM-3.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nb002-976-typeIII-ECRISM-4.csv   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nb003-976-typeIII-ECRISM-5.csv  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nb004-976-typeIII-ECRISM-6.csv </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nb005-976-typeIII-ECRISM-7.csv  </t>
+  </si>
+  <si>
+    <t>nb006-976-typeIII-ECRISM-8.csv</t>
+  </si>
+  <si>
+    <t>Bas</t>
+  </si>
+  <si>
+    <t>Rustenburg</t>
+  </si>
+  <si>
+    <t>bas.rustenburg@choderalab.org</t>
+  </si>
+  <si>
+    <t>nb007</t>
+  </si>
+  <si>
+    <t>nb007-976-typeIII-epik_sequential-1.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -849,13 +919,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1185,13 +1279,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L102"/>
+  <dimension ref="A1:L109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L102"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="F115" sqref="F115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="8" max="8" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -5048,8 +5146,275 @@
         <v>1516752678</v>
       </c>
     </row>
+    <row r="103" spans="1:12">
+      <c r="A103" t="s">
+        <v>78</v>
+      </c>
+      <c r="B103" t="s">
+        <v>79</v>
+      </c>
+      <c r="C103" t="s">
+        <v>80</v>
+      </c>
+      <c r="D103" t="s">
+        <v>81</v>
+      </c>
+      <c r="E103">
+        <v>1922</v>
+      </c>
+      <c r="F103">
+        <v>32601</v>
+      </c>
+      <c r="G103" t="s">
+        <v>266</v>
+      </c>
+      <c r="H103" t="s">
+        <v>273</v>
+      </c>
+      <c r="I103">
+        <v>976</v>
+      </c>
+      <c r="J103" t="s">
+        <v>18</v>
+      </c>
+      <c r="K103">
+        <v>0</v>
+      </c>
+      <c r="L103" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12">
+      <c r="A104" t="s">
+        <v>78</v>
+      </c>
+      <c r="B104" t="s">
+        <v>79</v>
+      </c>
+      <c r="C104" t="s">
+        <v>80</v>
+      </c>
+      <c r="D104" t="s">
+        <v>81</v>
+      </c>
+      <c r="E104">
+        <v>1923</v>
+      </c>
+      <c r="F104">
+        <v>32601</v>
+      </c>
+      <c r="G104" t="s">
+        <v>267</v>
+      </c>
+      <c r="H104" t="s">
+        <v>274</v>
+      </c>
+      <c r="I104">
+        <v>976</v>
+      </c>
+      <c r="J104" t="s">
+        <v>18</v>
+      </c>
+      <c r="K104">
+        <v>0</v>
+      </c>
+      <c r="L104" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12">
+      <c r="A105" t="s">
+        <v>78</v>
+      </c>
+      <c r="B105" t="s">
+        <v>79</v>
+      </c>
+      <c r="C105" t="s">
+        <v>80</v>
+      </c>
+      <c r="D105" t="s">
+        <v>81</v>
+      </c>
+      <c r="E105">
+        <v>1924</v>
+      </c>
+      <c r="F105">
+        <v>32601</v>
+      </c>
+      <c r="G105" t="s">
+        <v>268</v>
+      </c>
+      <c r="H105" t="s">
+        <v>275</v>
+      </c>
+      <c r="I105">
+        <v>976</v>
+      </c>
+      <c r="J105" t="s">
+        <v>18</v>
+      </c>
+      <c r="K105">
+        <v>0</v>
+      </c>
+      <c r="L105" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12">
+      <c r="A106" t="s">
+        <v>78</v>
+      </c>
+      <c r="B106" t="s">
+        <v>79</v>
+      </c>
+      <c r="C106" t="s">
+        <v>80</v>
+      </c>
+      <c r="D106" t="s">
+        <v>81</v>
+      </c>
+      <c r="E106">
+        <v>1925</v>
+      </c>
+      <c r="F106">
+        <v>32601</v>
+      </c>
+      <c r="G106" t="s">
+        <v>269</v>
+      </c>
+      <c r="H106" t="s">
+        <v>276</v>
+      </c>
+      <c r="I106">
+        <v>976</v>
+      </c>
+      <c r="J106" t="s">
+        <v>18</v>
+      </c>
+      <c r="K106">
+        <v>0</v>
+      </c>
+      <c r="L106" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12">
+      <c r="A107" t="s">
+        <v>78</v>
+      </c>
+      <c r="B107" t="s">
+        <v>79</v>
+      </c>
+      <c r="C107" t="s">
+        <v>80</v>
+      </c>
+      <c r="D107" t="s">
+        <v>81</v>
+      </c>
+      <c r="E107">
+        <v>1926</v>
+      </c>
+      <c r="F107">
+        <v>32601</v>
+      </c>
+      <c r="G107" t="s">
+        <v>270</v>
+      </c>
+      <c r="H107" t="s">
+        <v>277</v>
+      </c>
+      <c r="I107">
+        <v>976</v>
+      </c>
+      <c r="J107" t="s">
+        <v>18</v>
+      </c>
+      <c r="K107">
+        <v>0</v>
+      </c>
+      <c r="L107" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12">
+      <c r="A108" t="s">
+        <v>78</v>
+      </c>
+      <c r="B108" t="s">
+        <v>79</v>
+      </c>
+      <c r="C108" t="s">
+        <v>80</v>
+      </c>
+      <c r="D108" t="s">
+        <v>81</v>
+      </c>
+      <c r="E108">
+        <v>1927</v>
+      </c>
+      <c r="F108">
+        <v>32601</v>
+      </c>
+      <c r="G108" t="s">
+        <v>271</v>
+      </c>
+      <c r="H108" t="s">
+        <v>278</v>
+      </c>
+      <c r="I108">
+        <v>976</v>
+      </c>
+      <c r="J108" t="s">
+        <v>18</v>
+      </c>
+      <c r="K108">
+        <v>0</v>
+      </c>
+      <c r="L108" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12">
+      <c r="A109" t="s">
+        <v>279</v>
+      </c>
+      <c r="B109" t="s">
+        <v>280</v>
+      </c>
+      <c r="C109" t="s">
+        <v>281</v>
+      </c>
+      <c r="D109" t="s">
+        <v>71</v>
+      </c>
+      <c r="E109">
+        <v>1927</v>
+      </c>
+      <c r="F109">
+        <v>35000</v>
+      </c>
+      <c r="G109" t="s">
+        <v>282</v>
+      </c>
+      <c r="H109" t="s">
+        <v>283</v>
+      </c>
+      <c r="I109">
+        <v>976</v>
+      </c>
+      <c r="J109" t="s">
+        <v>18</v>
+      </c>
+      <c r="K109">
+        <v>0</v>
+      </c>
+      <c r="L109" t="s">
+        <v>272</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>